<commit_message>
Add the Iframe , refactoring the code, update data and add config file
</commit_message>
<xml_diff>
--- a/app/helper/excel/2020_02_21_covid19_country.xlsx
+++ b/app/helper/excel/2020_02_21_covid19_country.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="2020_02_21_covid19_country" sheetId="1" state="visible" r:id="rId2"/>
@@ -16,6 +16,7 @@
     <sheet name="2020_02_27_covid19" sheetId="6" state="visible" r:id="rId7"/>
     <sheet name="2020_02_29_covid19" sheetId="7" state="visible" r:id="rId8"/>
     <sheet name="2020_03_01_covid19" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="2020_03_02_covid19" sheetId="9" state="visible" r:id="rId10"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1338" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2058" uniqueCount="316">
   <si>
     <t xml:space="preserve">country</t>
   </si>
@@ -885,6 +886,96 @@
   </si>
   <si>
     <t xml:space="preserve">အာမေးနီးယား</t>
+  </si>
+  <si>
+    <t xml:space="preserve">၈၀၀၂၆</t>
+  </si>
+  <si>
+    <t xml:space="preserve">၂၀၂</t>
+  </si>
+  <si>
+    <t xml:space="preserve">၂၉၁၂</t>
+  </si>
+  <si>
+    <t xml:space="preserve">၃၂၃၃၉</t>
+  </si>
+  <si>
+    <t xml:space="preserve">၄၄၇၇၅</t>
+  </si>
+  <si>
+    <t xml:space="preserve">၇၁၁၀</t>
+  </si>
+  <si>
+    <t xml:space="preserve">၄၃၃၅</t>
+  </si>
+  <si>
+    <t xml:space="preserve">၅၉၉</t>
+  </si>
+  <si>
+    <t xml:space="preserve">၃၂၇၉</t>
+  </si>
+  <si>
+    <t xml:space="preserve">၁၇၀၄</t>
+  </si>
+  <si>
+    <t xml:space="preserve">၁၅၈၀</t>
+  </si>
+  <si>
+    <t xml:space="preserve">၁၅၀၁</t>
+  </si>
+  <si>
+    <t xml:space="preserve">၅၂၃</t>
+  </si>
+  <si>
+    <t xml:space="preserve">၁၁၄၄</t>
+  </si>
+  <si>
+    <t xml:space="preserve">၂၉၁</t>
+  </si>
+  <si>
+    <t xml:space="preserve">၂၅၆</t>
+  </si>
+  <si>
+    <t xml:space="preserve">၂၀၈</t>
+  </si>
+  <si>
+    <t xml:space="preserve">၁၅၀</t>
+  </si>
+  <si>
+    <t xml:space="preserve">၁၃၄</t>
+  </si>
+  <si>
+    <t xml:space="preserve">၁၃၀</t>
+  </si>
+  <si>
+    <t xml:space="preserve">၁၁၆</t>
+  </si>
+  <si>
+    <t xml:space="preserve">၈၈</t>
+  </si>
+  <si>
+    <t xml:space="preserve">၈၆</t>
+  </si>
+  <si>
+    <t xml:space="preserve">၈၄</t>
+  </si>
+  <si>
+    <t xml:space="preserve">အင်ဒိုနီးရှား</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ပေါ်တူဂီ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">အန်ဒိုရာ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">၆၉</t>
+  </si>
+  <si>
+    <t xml:space="preserve">၇၀</t>
+  </si>
+  <si>
+    <t xml:space="preserve">၇၂</t>
   </si>
 </sst>
 </file>
@@ -987,7 +1078,7 @@
       <selection pane="topLeft" activeCell="H11" activeCellId="0" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.42"/>
@@ -1479,7 +1570,7 @@
       <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="27.36"/>
@@ -2391,7 +2482,7 @@
       <selection pane="topLeft" activeCell="I15" activeCellId="0" sqref="I15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="27.58"/>
@@ -3407,7 +3498,7 @@
       <selection pane="topLeft" activeCell="M15" activeCellId="0" sqref="M15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -4523,7 +4614,7 @@
       <selection pane="topLeft" activeCell="J24" activeCellId="0" sqref="J24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -5717,7 +5808,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -7093,7 +7184,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -8699,8 +8790,2240 @@
   </sheetPr>
   <dimension ref="A1:J69"/>
   <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="131" zoomScaleNormal="131" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L19" activeCellId="0" sqref="L19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="I3" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="J3" s="0" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="I4" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="J4" s="0" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="I5" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="J5" s="0" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="I6" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="J6" s="0" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="G7" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="H7" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="I7" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="J7" s="0" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="G8" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="H8" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="I8" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="J8" s="0" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="G9" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="H9" s="0" t="s">
+        <v>164</v>
+      </c>
+      <c r="I9" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="J9" s="0" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="G10" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="H10" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="I10" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="J10" s="0" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="F11" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="G11" s="0" t="s">
+        <v>173</v>
+      </c>
+      <c r="H11" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="I11" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="J11" s="0" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>174</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>175</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="F12" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="G12" s="0" t="s">
+        <v>176</v>
+      </c>
+      <c r="H12" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="I12" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="J12" s="0" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>178</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="F13" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="G13" s="0" t="s">
+        <v>179</v>
+      </c>
+      <c r="H13" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="I13" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="J13" s="0" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>182</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>183</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="F14" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="G14" s="0" t="s">
+        <v>183</v>
+      </c>
+      <c r="H14" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="I14" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="J14" s="0" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>185</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>186</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="F15" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="G15" s="0" t="s">
+        <v>186</v>
+      </c>
+      <c r="H15" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="I15" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="J15" s="0" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>187</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>188</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>189</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="F16" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="G16" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="H16" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="I16" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="J16" s="0" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>190</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>191</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="F17" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="G17" s="0" t="s">
+        <v>192</v>
+      </c>
+      <c r="H17" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="I17" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="J17" s="0" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>193</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>194</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="F18" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="G18" s="0" t="s">
+        <v>192</v>
+      </c>
+      <c r="H18" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="I18" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="J18" s="0" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>195</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>196</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>197</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="E19" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="F19" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="G19" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="H19" s="0" t="s">
+        <v>198</v>
+      </c>
+      <c r="I19" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="J19" s="0" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>199</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>200</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="E20" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="F20" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="G20" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="H20" s="0" t="s">
+        <v>187</v>
+      </c>
+      <c r="I20" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="J20" s="0" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>201</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>202</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="E21" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="F21" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="G21" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="H21" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="I21" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="J21" s="0" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>203</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>201</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="E22" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="F22" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="G22" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="H22" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="I22" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="J22" s="0" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>198</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>204</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="E23" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="F23" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="G23" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="H23" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="I23" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="J23" s="0" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>205</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>206</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="E24" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="F24" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="G24" s="0" t="s">
+        <v>195</v>
+      </c>
+      <c r="H24" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="I24" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="J24" s="0" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>207</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>208</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>193</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="E25" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="F25" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="G25" s="0" t="s">
+        <v>193</v>
+      </c>
+      <c r="H25" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="I25" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="J25" s="0" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>210</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>211</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="D26" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="E26" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="F26" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="G26" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="H26" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="I26" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="J26" s="0" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>200</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>212</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="E27" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="F27" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="G27" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="H27" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="I27" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="J27" s="0" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>192</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>213</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="E28" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="F28" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="G28" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="H28" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="I28" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="J28" s="0" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>214</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>215</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="D29" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="E29" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="F29" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="G29" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="H29" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="I29" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="J29" s="0" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>197</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>216</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="D30" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="E30" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="F30" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="G30" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="H30" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="I30" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="J30" s="0" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="B31" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="C31" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="D31" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="E31" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="F31" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="G31" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="H31" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="I31" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="J31" s="0" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="B32" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="C32" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="D32" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="E32" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="F32" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="G32" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="H32" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="I32" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="J32" s="0" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>220</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="D33" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="E33" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="F33" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="G33" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="H33" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="I33" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="J33" s="0" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>221</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>222</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="D34" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="E34" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="F34" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="G34" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="H34" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="I34" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="J34" s="0" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="B35" s="0" t="s">
+        <v>223</v>
+      </c>
+      <c r="C35" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="D35" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="E35" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="F35" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="G35" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="H35" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="I35" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="J35" s="0" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="B36" s="0" t="s">
+        <v>224</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="D36" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="E36" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="F36" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="G36" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="H36" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="I36" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="J36" s="0" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="B37" s="0" t="s">
+        <v>225</v>
+      </c>
+      <c r="C37" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="D37" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="E37" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="F37" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="G37" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="H37" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="I37" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="J37" s="0" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>226</v>
+      </c>
+      <c r="B38" s="0" t="s">
+        <v>227</v>
+      </c>
+      <c r="C38" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="D38" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="E38" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="F38" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="G38" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="H38" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="I38" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="J38" s="0" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>228</v>
+      </c>
+      <c r="B39" s="0" t="s">
+        <v>229</v>
+      </c>
+      <c r="C39" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="D39" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="E39" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="F39" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="G39" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="H39" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="I39" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="J39" s="0" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
+        <v>230</v>
+      </c>
+      <c r="B40" s="0" t="s">
+        <v>231</v>
+      </c>
+      <c r="C40" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="D40" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="E40" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="F40" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="G40" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="H40" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="I40" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="J40" s="0" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
+        <v>191</v>
+      </c>
+      <c r="B41" s="0" t="s">
+        <v>232</v>
+      </c>
+      <c r="C41" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="D41" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="E41" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="F41" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="G41" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="H41" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="I41" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="J41" s="0" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
+        <v>233</v>
+      </c>
+      <c r="B42" s="0" t="s">
+        <v>234</v>
+      </c>
+      <c r="C42" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="D42" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="E42" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="F42" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="G42" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="H42" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="I42" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="J42" s="0" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
+        <v>189</v>
+      </c>
+      <c r="B43" s="0" t="s">
+        <v>235</v>
+      </c>
+      <c r="C43" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="D43" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="E43" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="F43" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="G43" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="H43" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="I43" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="J43" s="0" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="s">
+        <v>236</v>
+      </c>
+      <c r="B44" s="0" t="s">
+        <v>237</v>
+      </c>
+      <c r="C44" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="D44" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="E44" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="F44" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="G44" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="H44" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="I44" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="J44" s="0" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
+        <v>238</v>
+      </c>
+      <c r="B45" s="0" t="s">
+        <v>239</v>
+      </c>
+      <c r="C45" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="D45" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="E45" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="F45" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="G45" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="H45" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="I45" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="J45" s="0" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
+        <v>240</v>
+      </c>
+      <c r="B46" s="0" t="s">
+        <v>241</v>
+      </c>
+      <c r="C46" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="D46" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="E46" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="F46" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="G46" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="H46" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="I46" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="J46" s="0" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="s">
+        <v>186</v>
+      </c>
+      <c r="B47" s="0" t="s">
+        <v>242</v>
+      </c>
+      <c r="C47" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="D47" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="E47" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="F47" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="G47" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="H47" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="I47" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="J47" s="0" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="s">
+        <v>183</v>
+      </c>
+      <c r="B48" s="0" t="s">
+        <v>244</v>
+      </c>
+      <c r="C48" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="D48" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="E48" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="F48" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="G48" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="H48" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="I48" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="J48" s="0" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="s">
+        <v>245</v>
+      </c>
+      <c r="B49" s="0" t="s">
+        <v>246</v>
+      </c>
+      <c r="C49" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="D49" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="E49" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="F49" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="G49" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="H49" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="I49" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="J49" s="0" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="s">
+        <v>248</v>
+      </c>
+      <c r="B50" s="0" t="s">
+        <v>249</v>
+      </c>
+      <c r="C50" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="D50" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="E50" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="F50" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="G50" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="H50" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="I50" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="J50" s="0" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="B51" s="0" t="s">
+        <v>250</v>
+      </c>
+      <c r="C51" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="D51" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="E51" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="F51" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="G51" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="H51" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="I51" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="J51" s="0" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="s">
+        <v>251</v>
+      </c>
+      <c r="B52" s="0" t="s">
+        <v>252</v>
+      </c>
+      <c r="C52" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="D52" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="E52" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="F52" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="G52" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="H52" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="I52" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="J52" s="0" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0" t="s">
+        <v>253</v>
+      </c>
+      <c r="B53" s="0" t="s">
+        <v>254</v>
+      </c>
+      <c r="C53" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="D53" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="E53" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="F53" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="G53" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="H53" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="I53" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="J53" s="0" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="0" t="s">
+        <v>255</v>
+      </c>
+      <c r="B54" s="0" t="s">
+        <v>256</v>
+      </c>
+      <c r="C54" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="D54" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="E54" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="F54" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="G54" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="H54" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="I54" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="J54" s="0" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="B55" s="0" t="s">
+        <v>258</v>
+      </c>
+      <c r="C55" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="D55" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="E55" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="F55" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="G55" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="H55" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="I55" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="J55" s="0" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="0" t="s">
+        <v>259</v>
+      </c>
+      <c r="B56" s="0" t="s">
+        <v>260</v>
+      </c>
+      <c r="C56" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="D56" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="E56" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="F56" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="G56" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="H56" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="I56" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="J56" s="0" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0" t="s">
+        <v>261</v>
+      </c>
+      <c r="B57" s="0" t="s">
+        <v>262</v>
+      </c>
+      <c r="C57" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="D57" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="E57" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="F57" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="G57" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="H57" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="I57" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="J57" s="0" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="0" t="s">
+        <v>264</v>
+      </c>
+      <c r="B58" s="0" t="s">
+        <v>265</v>
+      </c>
+      <c r="C58" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="D58" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="E58" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="F58" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="G58" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="H58" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="I58" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="J58" s="0" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="0" t="s">
+        <v>266</v>
+      </c>
+      <c r="B59" s="0" t="s">
+        <v>267</v>
+      </c>
+      <c r="C59" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="D59" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="E59" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="F59" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="G59" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="H59" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="I59" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="J59" s="0" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="0" t="s">
+        <v>268</v>
+      </c>
+      <c r="B60" s="0" t="s">
+        <v>269</v>
+      </c>
+      <c r="C60" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="D60" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="E60" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="F60" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="G60" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="H60" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="I60" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="J60" s="0" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="0" t="s">
+        <v>270</v>
+      </c>
+      <c r="B61" s="0" t="s">
+        <v>271</v>
+      </c>
+      <c r="C61" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="D61" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="E61" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="F61" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="G61" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="H61" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="I61" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="J61" s="0" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="0" t="s">
+        <v>179</v>
+      </c>
+      <c r="B62" s="0" t="s">
+        <v>272</v>
+      </c>
+      <c r="C62" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="D62" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="E62" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="F62" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="G62" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="H62" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="I62" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="J62" s="0" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="0" t="s">
+        <v>173</v>
+      </c>
+      <c r="B63" s="0" t="s">
+        <v>273</v>
+      </c>
+      <c r="C63" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="D63" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="E63" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="F63" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="G63" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="H63" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="I63" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="J63" s="0" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="0" t="s">
+        <v>274</v>
+      </c>
+      <c r="B64" s="0" t="s">
+        <v>275</v>
+      </c>
+      <c r="C64" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="D64" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="E64" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="F64" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="G64" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="H64" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="I64" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="J64" s="0" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="0" t="s">
+        <v>276</v>
+      </c>
+      <c r="B65" s="0" t="s">
+        <v>277</v>
+      </c>
+      <c r="C65" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="D65" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="E65" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="F65" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="G65" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="H65" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="I65" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="J65" s="0" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="0" t="s">
+        <v>278</v>
+      </c>
+      <c r="B66" s="0" t="s">
+        <v>279</v>
+      </c>
+      <c r="C66" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="D66" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="E66" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="F66" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="G66" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="H66" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="I66" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="J66" s="0" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="0" t="s">
+        <v>280</v>
+      </c>
+      <c r="B67" s="0" t="s">
+        <v>281</v>
+      </c>
+      <c r="C67" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="D67" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="E67" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="F67" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="G67" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="H67" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="I67" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="J67" s="0" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="0" t="s">
+        <v>282</v>
+      </c>
+      <c r="B68" s="0" t="s">
+        <v>283</v>
+      </c>
+      <c r="C68" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="D68" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="E68" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="F68" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="G68" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="H68" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="I68" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="J68" s="0" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="0" t="s">
+        <v>284</v>
+      </c>
+      <c r="B69" s="0" t="s">
+        <v>285</v>
+      </c>
+      <c r="C69" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="D69" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="E69" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="F69" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="G69" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="H69" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="I69" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="J69" s="0" t="s">
+        <v>135</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:J72"/>
+  <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="131" zoomScaleNormal="131" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L19" activeCellId="0" sqref="L19"/>
+      <selection pane="topLeft" activeCell="K13" activeCellId="0" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8745,25 +11068,25 @@
         <v>108</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>109</v>
+        <v>286</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>110</v>
+        <v>287</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>111</v>
+        <v>288</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>112</v>
+        <v>189</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>113</v>
+        <v>289</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>114</v>
+        <v>290</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>115</v>
+        <v>291</v>
       </c>
       <c r="J2" s="0" t="s">
         <v>116</v>
@@ -8777,25 +11100,25 @@
         <v>118</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>119</v>
+        <v>292</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>120</v>
+        <v>293</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>121</v>
+        <v>200</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>122</v>
+        <v>131</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>123</v>
+        <v>294</v>
       </c>
       <c r="H3" s="0" t="s">
         <v>124</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>125</v>
+        <v>192</v>
       </c>
       <c r="J3" s="0" t="s">
         <v>116</v>
@@ -8809,19 +11132,19 @@
         <v>127</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>128</v>
+        <v>295</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>130</v>
+        <v>233</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>131</v>
+        <v>143</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>132</v>
+        <v>296</v>
       </c>
       <c r="H4" s="0" t="s">
         <v>133</v>
@@ -8841,22 +11164,22 @@
         <v>136</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>137</v>
+        <v>297</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>138</v>
+        <v>298</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>139</v>
+        <v>280</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>140</v>
+        <v>170</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>141</v>
+        <v>299</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>142</v>
+        <v>300</v>
       </c>
       <c r="I5" s="0" t="s">
         <v>143</v>
@@ -8905,22 +11228,22 @@
         <v>151</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>152</v>
+        <v>301</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="E7" s="0" t="s">
         <v>150</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>107</v>
+        <v>143</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>153</v>
+        <v>302</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>154</v>
+        <v>189</v>
       </c>
       <c r="I7" s="0" t="s">
         <v>155</v>
@@ -8937,10 +11260,10 @@
         <v>156</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>157</v>
+        <v>303</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>158</v>
+        <v>287</v>
       </c>
       <c r="E8" s="0" t="s">
         <v>143</v>
@@ -8949,7 +11272,7 @@
         <v>143</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>159</v>
+        <v>304</v>
       </c>
       <c r="H8" s="0" t="s">
         <v>160</v>
@@ -8963,66 +11286,66 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>163</v>
+        <v>305</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>122</v>
+        <v>143</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>143</v>
+        <v>117</v>
       </c>
       <c r="F9" s="0" t="s">
         <v>143</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>154</v>
+        <v>306</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>146</v>
+        <v>166</v>
       </c>
       <c r="J9" s="0" t="s">
-        <v>165</v>
+        <v>135</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>122</v>
+        <v>143</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>117</v>
+        <v>143</v>
       </c>
       <c r="F10" s="0" t="s">
         <v>143</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>166</v>
+        <v>146</v>
       </c>
       <c r="J10" s="0" t="s">
-        <v>135</v>
+        <v>165</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9036,7 +11359,7 @@
         <v>172</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>131</v>
+        <v>143</v>
       </c>
       <c r="E11" s="0" t="s">
         <v>117</v>
@@ -9062,31 +11385,31 @@
         <v>140</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>175</v>
+        <v>307</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>121</v>
+        <v>181</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>143</v>
+        <v>117</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>143</v>
+        <v>107</v>
       </c>
       <c r="G12" s="0" t="s">
         <v>176</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>117</v>
+        <v>166</v>
       </c>
       <c r="I12" s="0" t="s">
-        <v>126</v>
+        <v>161</v>
       </c>
       <c r="J12" s="0" t="s">
-        <v>135</v>
+        <v>180</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9094,31 +11417,31 @@
         <v>170</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>178</v>
+        <v>308</v>
       </c>
       <c r="D13" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="F13" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="G13" s="0" t="s">
+        <v>309</v>
+      </c>
+      <c r="H13" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="I13" s="0" t="s">
         <v>126</v>
       </c>
-      <c r="E13" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="F13" s="0" t="s">
-        <v>143</v>
-      </c>
-      <c r="G13" s="0" t="s">
-        <v>179</v>
-      </c>
-      <c r="H13" s="0" t="s">
-        <v>166</v>
-      </c>
-      <c r="I13" s="0" t="s">
-        <v>107</v>
-      </c>
       <c r="J13" s="0" t="s">
-        <v>180</v>
+        <v>135</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9126,13 +11449,13 @@
         <v>181</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>183</v>
+        <v>261</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>150</v>
+        <v>125</v>
       </c>
       <c r="E14" s="0" t="s">
         <v>143</v>
@@ -9141,7 +11464,7 @@
         <v>143</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>183</v>
+        <v>261</v>
       </c>
       <c r="H14" s="0" t="s">
         <v>143</v>
@@ -9158,13 +11481,13 @@
         <v>184</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>107</v>
+        <v>143</v>
       </c>
       <c r="E15" s="0" t="s">
         <v>143</v>
@@ -9173,7 +11496,7 @@
         <v>143</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="H15" s="0" t="s">
         <v>143</v>
@@ -9193,10 +11516,10 @@
         <v>188</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>189</v>
+        <v>236</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>143</v>
+        <v>107</v>
       </c>
       <c r="E16" s="0" t="s">
         <v>107</v>
@@ -9205,7 +11528,7 @@
         <v>107</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>140</v>
+        <v>170</v>
       </c>
       <c r="H16" s="0" t="s">
         <v>124</v>
@@ -9228,7 +11551,7 @@
         <v>191</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>107</v>
+        <v>143</v>
       </c>
       <c r="E17" s="0" t="s">
         <v>107</v>
@@ -9257,10 +11580,10 @@
         <v>194</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>112</v>
+        <v>148</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>170</v>
+        <v>143</v>
       </c>
       <c r="E18" s="0" t="s">
         <v>143</v>
@@ -9269,7 +11592,7 @@
         <v>143</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>192</v>
+        <v>214</v>
       </c>
       <c r="H18" s="0" t="s">
         <v>161</v>
@@ -9286,31 +11609,31 @@
         <v>195</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>197</v>
+        <v>124</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>122</v>
+        <v>107</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>143</v>
+        <v>107</v>
       </c>
       <c r="F19" s="0" t="s">
         <v>143</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>146</v>
+        <v>184</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
       <c r="I19" s="0" t="s">
         <v>143</v>
       </c>
       <c r="J19" s="0" t="s">
-        <v>165</v>
+        <v>199</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9318,31 +11641,31 @@
         <v>155</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>107</v>
+        <v>143</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>107</v>
+        <v>143</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>107</v>
+        <v>143</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>125</v>
+        <v>146</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>187</v>
+        <v>198</v>
       </c>
       <c r="I20" s="0" t="s">
         <v>143</v>
       </c>
       <c r="J20" s="0" t="s">
-        <v>199</v>
+        <v>165</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9350,10 +11673,10 @@
         <v>201</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>121</v>
+        <v>207</v>
       </c>
       <c r="D21" s="0" t="s">
         <v>143</v>
@@ -9365,16 +11688,16 @@
         <v>143</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>160</v>
+        <v>201</v>
       </c>
       <c r="H21" s="0" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="I21" s="0" t="s">
-        <v>117</v>
+        <v>143</v>
       </c>
       <c r="J21" s="0" t="s">
-        <v>165</v>
+        <v>180</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9382,10 +11705,10 @@
         <v>121</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
       <c r="D22" s="0" t="s">
         <v>143</v>
@@ -9397,16 +11720,16 @@
         <v>143</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>160</v>
+        <v>205</v>
       </c>
       <c r="H22" s="0" t="s">
-        <v>122</v>
+        <v>107</v>
       </c>
       <c r="I22" s="0" t="s">
         <v>143</v>
       </c>
       <c r="J22" s="0" t="s">
-        <v>180</v>
+        <v>135</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9417,10 +11740,10 @@
         <v>204</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>155</v>
+        <v>121</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>150</v>
+        <v>117</v>
       </c>
       <c r="E23" s="0" t="s">
         <v>143</v>
@@ -9429,7 +11752,7 @@
         <v>143</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>155</v>
+        <v>121</v>
       </c>
       <c r="H23" s="0" t="s">
         <v>143</v>
@@ -9446,10 +11769,10 @@
         <v>205</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>155</v>
+        <v>121</v>
       </c>
       <c r="D24" s="0" t="s">
         <v>143</v>
@@ -9461,16 +11784,16 @@
         <v>143</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>195</v>
+        <v>160</v>
       </c>
       <c r="H24" s="0" t="s">
-        <v>107</v>
+        <v>131</v>
       </c>
       <c r="I24" s="0" t="s">
-        <v>143</v>
+        <v>117</v>
       </c>
       <c r="J24" s="0" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9481,10 +11804,10 @@
         <v>208</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>193</v>
+        <v>155</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>117</v>
+        <v>143</v>
       </c>
       <c r="E25" s="0" t="s">
         <v>143</v>
@@ -9493,7 +11816,7 @@
         <v>143</v>
       </c>
       <c r="G25" s="0" t="s">
-        <v>193</v>
+        <v>155</v>
       </c>
       <c r="H25" s="0" t="s">
         <v>143</v>
@@ -9545,10 +11868,10 @@
         <v>212</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>122</v>
+        <v>107</v>
       </c>
       <c r="E27" s="0" t="s">
         <v>143</v>
@@ -9557,7 +11880,7 @@
         <v>143</v>
       </c>
       <c r="G27" s="0" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="H27" s="0" t="s">
         <v>143</v>
@@ -9577,7 +11900,7 @@
         <v>213</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="D28" s="0" t="s">
         <v>143</v>
@@ -9589,7 +11912,7 @@
         <v>143</v>
       </c>
       <c r="G28" s="0" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="H28" s="0" t="s">
         <v>143</v>
@@ -9638,13 +11961,13 @@
         <v>197</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="C30" s="0" t="s">
         <v>125</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>126</v>
+        <v>143</v>
       </c>
       <c r="E30" s="0" t="s">
         <v>143</v>
@@ -9653,10 +11976,10 @@
         <v>143</v>
       </c>
       <c r="G30" s="0" t="s">
-        <v>125</v>
+        <v>166</v>
       </c>
       <c r="H30" s="0" t="s">
-        <v>143</v>
+        <v>107</v>
       </c>
       <c r="I30" s="0" t="s">
         <v>143</v>
@@ -9670,7 +11993,7 @@
         <v>124</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C31" s="0" t="s">
         <v>125</v>
@@ -9691,10 +12014,10 @@
         <v>143</v>
       </c>
       <c r="I31" s="0" t="s">
-        <v>107</v>
+        <v>143</v>
       </c>
       <c r="J31" s="0" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9702,28 +12025,28 @@
         <v>218</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>146</v>
+        <v>125</v>
       </c>
       <c r="D32" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="E32" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="F32" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="G32" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="H32" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="I32" s="0" t="s">
         <v>107</v>
-      </c>
-      <c r="E32" s="0" t="s">
-        <v>143</v>
-      </c>
-      <c r="F32" s="0" t="s">
-        <v>143</v>
-      </c>
-      <c r="G32" s="0" t="s">
-        <v>146</v>
-      </c>
-      <c r="H32" s="0" t="s">
-        <v>143</v>
-      </c>
-      <c r="I32" s="0" t="s">
-        <v>143</v>
       </c>
       <c r="J32" s="0" t="s">
         <v>135</v>
@@ -9734,16 +12057,16 @@
         <v>154</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>220</v>
+        <v>281</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>146</v>
+        <v>161</v>
       </c>
       <c r="D33" s="0" t="s">
         <v>143</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>143</v>
+        <v>107</v>
       </c>
       <c r="F33" s="0" t="s">
         <v>143</v>
@@ -9755,7 +12078,7 @@
         <v>143</v>
       </c>
       <c r="I33" s="0" t="s">
-        <v>143</v>
+        <v>107</v>
       </c>
       <c r="J33" s="0" t="s">
         <v>135</v>
@@ -9766,31 +12089,31 @@
         <v>221</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>222</v>
+        <v>244</v>
       </c>
       <c r="C34" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="D34" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="E34" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="F34" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="G34" s="0" t="s">
         <v>146</v>
       </c>
-      <c r="D34" s="0" t="s">
-        <v>143</v>
-      </c>
-      <c r="E34" s="0" t="s">
-        <v>143</v>
-      </c>
-      <c r="F34" s="0" t="s">
-        <v>143</v>
-      </c>
-      <c r="G34" s="0" t="s">
-        <v>150</v>
-      </c>
       <c r="H34" s="0" t="s">
-        <v>143</v>
+        <v>107</v>
       </c>
       <c r="I34" s="0" t="s">
         <v>143</v>
       </c>
       <c r="J34" s="0" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9798,13 +12121,13 @@
         <v>130</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>150</v>
+        <v>161</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>126</v>
+        <v>107</v>
       </c>
       <c r="E35" s="0" t="s">
         <v>143</v>
@@ -9813,10 +12136,10 @@
         <v>143</v>
       </c>
       <c r="G35" s="0" t="s">
-        <v>131</v>
+        <v>161</v>
       </c>
       <c r="H35" s="0" t="s">
-        <v>107</v>
+        <v>143</v>
       </c>
       <c r="I35" s="0" t="s">
         <v>143</v>
@@ -9830,10 +12153,10 @@
         <v>112</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="D36" s="0" t="s">
         <v>143</v>
@@ -9845,7 +12168,7 @@
         <v>143</v>
       </c>
       <c r="G36" s="0" t="s">
-        <v>131</v>
+        <v>146</v>
       </c>
       <c r="H36" s="0" t="s">
         <v>143</v>
@@ -9854,7 +12177,7 @@
         <v>143</v>
       </c>
       <c r="J36" s="0" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9862,10 +12185,10 @@
         <v>148</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>225</v>
+        <v>258</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>122</v>
+        <v>150</v>
       </c>
       <c r="D37" s="0" t="s">
         <v>143</v>
@@ -9877,16 +12200,16 @@
         <v>143</v>
       </c>
       <c r="G37" s="0" t="s">
-        <v>122</v>
+        <v>150</v>
       </c>
       <c r="H37" s="0" t="s">
         <v>143</v>
       </c>
       <c r="I37" s="0" t="s">
-        <v>143</v>
+        <v>107</v>
       </c>
       <c r="J37" s="0" t="s">
-        <v>180</v>
+        <v>243</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9894,13 +12217,13 @@
         <v>226</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>122</v>
+        <v>150</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>143</v>
+        <v>126</v>
       </c>
       <c r="E38" s="0" t="s">
         <v>143</v>
@@ -9909,16 +12232,16 @@
         <v>143</v>
       </c>
       <c r="G38" s="0" t="s">
-        <v>122</v>
+        <v>131</v>
       </c>
       <c r="H38" s="0" t="s">
-        <v>143</v>
+        <v>107</v>
       </c>
       <c r="I38" s="0" t="s">
         <v>143</v>
       </c>
       <c r="J38" s="0" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9926,31 +12249,31 @@
         <v>228</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>126</v>
+        <v>150</v>
       </c>
       <c r="D39" s="0" t="s">
         <v>143</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>107</v>
+        <v>143</v>
       </c>
       <c r="F39" s="0" t="s">
         <v>143</v>
       </c>
       <c r="G39" s="0" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
       <c r="H39" s="0" t="s">
-        <v>117</v>
+        <v>143</v>
       </c>
       <c r="I39" s="0" t="s">
         <v>143</v>
       </c>
       <c r="J39" s="0" t="s">
-        <v>165</v>
+        <v>144</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9958,31 +12281,31 @@
         <v>230</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>231</v>
+        <v>237</v>
       </c>
       <c r="C40" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="D40" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="E40" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="F40" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="G40" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="H40" s="0" t="s">
         <v>126</v>
       </c>
-      <c r="D40" s="0" t="s">
-        <v>143</v>
-      </c>
-      <c r="E40" s="0" t="s">
-        <v>143</v>
-      </c>
-      <c r="F40" s="0" t="s">
-        <v>143</v>
-      </c>
-      <c r="G40" s="0" t="s">
-        <v>126</v>
-      </c>
-      <c r="H40" s="0" t="s">
-        <v>143</v>
-      </c>
       <c r="I40" s="0" t="s">
         <v>143</v>
       </c>
       <c r="J40" s="0" t="s">
-        <v>135</v>
+        <v>116</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9990,13 +12313,13 @@
         <v>191</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>126</v>
+        <v>143</v>
       </c>
       <c r="E41" s="0" t="s">
         <v>143</v>
@@ -10005,7 +12328,7 @@
         <v>143</v>
       </c>
       <c r="G41" s="0" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="H41" s="0" t="s">
         <v>143</v>
@@ -10014,7 +12337,7 @@
         <v>143</v>
       </c>
       <c r="J41" s="0" t="s">
-        <v>135</v>
+        <v>180</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10025,7 +12348,7 @@
         <v>234</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="D42" s="0" t="s">
         <v>143</v>
@@ -10037,7 +12360,7 @@
         <v>143</v>
       </c>
       <c r="G42" s="0" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="H42" s="0" t="s">
         <v>143</v>
@@ -10054,10 +12377,10 @@
         <v>189</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="D43" s="0" t="s">
         <v>143</v>
@@ -10069,7 +12392,7 @@
         <v>143</v>
       </c>
       <c r="G43" s="0" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="H43" s="0" t="s">
         <v>143</v>
@@ -10078,7 +12401,7 @@
         <v>143</v>
       </c>
       <c r="J43" s="0" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10086,7 +12409,7 @@
         <v>236</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
       <c r="C44" s="0" t="s">
         <v>126</v>
@@ -10095,7 +12418,7 @@
         <v>143</v>
       </c>
       <c r="E44" s="0" t="s">
-        <v>143</v>
+        <v>107</v>
       </c>
       <c r="F44" s="0" t="s">
         <v>143</v>
@@ -10104,13 +12427,13 @@
         <v>143</v>
       </c>
       <c r="H44" s="0" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="I44" s="0" t="s">
         <v>143</v>
       </c>
       <c r="J44" s="0" t="s">
-        <v>116</v>
+        <v>165</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10118,13 +12441,13 @@
         <v>238</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="C45" s="0" t="s">
         <v>126</v>
       </c>
       <c r="D45" s="0" t="s">
-        <v>117</v>
+        <v>143</v>
       </c>
       <c r="E45" s="0" t="s">
         <v>143</v>
@@ -10142,7 +12465,7 @@
         <v>143</v>
       </c>
       <c r="J45" s="0" t="s">
-        <v>144</v>
+        <v>243</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10150,7 +12473,7 @@
         <v>240</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>241</v>
+        <v>231</v>
       </c>
       <c r="C46" s="0" t="s">
         <v>126</v>
@@ -10165,10 +12488,10 @@
         <v>143</v>
       </c>
       <c r="G46" s="0" t="s">
-        <v>117</v>
+        <v>126</v>
       </c>
       <c r="H46" s="0" t="s">
-        <v>107</v>
+        <v>143</v>
       </c>
       <c r="I46" s="0" t="s">
         <v>143</v>
@@ -10182,13 +12505,13 @@
         <v>186</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>242</v>
+        <v>232</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>117</v>
+        <v>126</v>
       </c>
       <c r="D47" s="0" t="s">
-        <v>107</v>
+        <v>143</v>
       </c>
       <c r="E47" s="0" t="s">
         <v>143</v>
@@ -10197,7 +12520,7 @@
         <v>143</v>
       </c>
       <c r="G47" s="0" t="s">
-        <v>117</v>
+        <v>126</v>
       </c>
       <c r="H47" s="0" t="s">
         <v>143</v>
@@ -10206,7 +12529,7 @@
         <v>143</v>
       </c>
       <c r="J47" s="0" t="s">
-        <v>243</v>
+        <v>135</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10214,13 +12537,13 @@
         <v>183</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>117</v>
+        <v>126</v>
       </c>
       <c r="D48" s="0" t="s">
-        <v>107</v>
+        <v>143</v>
       </c>
       <c r="E48" s="0" t="s">
         <v>143</v>
@@ -10229,10 +12552,10 @@
         <v>143</v>
       </c>
       <c r="G48" s="0" t="s">
-        <v>107</v>
+        <v>126</v>
       </c>
       <c r="H48" s="0" t="s">
-        <v>107</v>
+        <v>143</v>
       </c>
       <c r="I48" s="0" t="s">
         <v>143</v>
@@ -10246,10 +12569,10 @@
         <v>245</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>246</v>
+        <v>265</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>117</v>
+        <v>126</v>
       </c>
       <c r="D49" s="0" t="s">
         <v>143</v>
@@ -10261,7 +12584,7 @@
         <v>143</v>
       </c>
       <c r="G49" s="0" t="s">
-        <v>117</v>
+        <v>126</v>
       </c>
       <c r="H49" s="0" t="s">
         <v>143</v>
@@ -10270,7 +12593,7 @@
         <v>143</v>
       </c>
       <c r="J49" s="0" t="s">
-        <v>247</v>
+        <v>135</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10278,14 +12601,14 @@
         <v>248</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>249</v>
+        <v>239</v>
       </c>
       <c r="C50" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="D50" s="0" t="s">
         <v>117</v>
       </c>
-      <c r="D50" s="0" t="s">
-        <v>143</v>
-      </c>
       <c r="E50" s="0" t="s">
         <v>143</v>
       </c>
@@ -10293,16 +12616,16 @@
         <v>143</v>
       </c>
       <c r="G50" s="0" t="s">
-        <v>143</v>
+        <v>126</v>
       </c>
       <c r="H50" s="0" t="s">
-        <v>117</v>
+        <v>143</v>
       </c>
       <c r="I50" s="0" t="s">
         <v>143</v>
       </c>
       <c r="J50" s="0" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10310,31 +12633,31 @@
         <v>158</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>250</v>
+        <v>241</v>
       </c>
       <c r="C51" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="D51" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="E51" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="F51" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="G51" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="H51" s="0" t="s">
         <v>107</v>
       </c>
-      <c r="D51" s="0" t="s">
-        <v>143</v>
-      </c>
-      <c r="E51" s="0" t="s">
-        <v>143</v>
-      </c>
-      <c r="F51" s="0" t="s">
-        <v>143</v>
-      </c>
-      <c r="G51" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="H51" s="0" t="s">
-        <v>143</v>
-      </c>
       <c r="I51" s="0" t="s">
         <v>143</v>
       </c>
       <c r="J51" s="0" t="s">
-        <v>116</v>
+        <v>135</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10342,13 +12665,13 @@
         <v>251</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="C52" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="D52" s="0" t="s">
         <v>107</v>
-      </c>
-      <c r="D52" s="0" t="s">
-        <v>143</v>
       </c>
       <c r="E52" s="0" t="s">
         <v>143</v>
@@ -10360,7 +12683,7 @@
         <v>107</v>
       </c>
       <c r="H52" s="0" t="s">
-        <v>143</v>
+        <v>117</v>
       </c>
       <c r="I52" s="0" t="s">
         <v>143</v>
@@ -10374,10 +12697,10 @@
         <v>253</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>107</v>
+        <v>117</v>
       </c>
       <c r="D53" s="0" t="s">
         <v>143</v>
@@ -10389,16 +12712,16 @@
         <v>143</v>
       </c>
       <c r="G53" s="0" t="s">
-        <v>143</v>
+        <v>117</v>
       </c>
       <c r="H53" s="0" t="s">
-        <v>107</v>
+        <v>143</v>
       </c>
       <c r="I53" s="0" t="s">
         <v>143</v>
       </c>
       <c r="J53" s="0" t="s">
-        <v>165</v>
+        <v>247</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10406,13 +12729,13 @@
         <v>255</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>256</v>
+        <v>260</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>107</v>
+        <v>117</v>
       </c>
       <c r="D54" s="0" t="s">
-        <v>107</v>
+        <v>143</v>
       </c>
       <c r="E54" s="0" t="s">
         <v>143</v>
@@ -10421,16 +12744,16 @@
         <v>143</v>
       </c>
       <c r="G54" s="0" t="s">
-        <v>107</v>
+        <v>143</v>
       </c>
       <c r="H54" s="0" t="s">
-        <v>143</v>
+        <v>117</v>
       </c>
       <c r="I54" s="0" t="s">
         <v>143</v>
       </c>
       <c r="J54" s="0" t="s">
-        <v>257</v>
+        <v>243</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10438,13 +12761,13 @@
         <v>139</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>258</v>
+        <v>310</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>107</v>
+        <v>117</v>
       </c>
       <c r="D55" s="0" t="s">
-        <v>143</v>
+        <v>117</v>
       </c>
       <c r="E55" s="0" t="s">
         <v>143</v>
@@ -10453,16 +12776,16 @@
         <v>143</v>
       </c>
       <c r="G55" s="0" t="s">
-        <v>107</v>
+        <v>117</v>
       </c>
       <c r="H55" s="0" t="s">
         <v>143</v>
       </c>
       <c r="I55" s="0" t="s">
-        <v>107</v>
+        <v>143</v>
       </c>
       <c r="J55" s="0" t="s">
-        <v>243</v>
+        <v>165</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10470,13 +12793,13 @@
         <v>259</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>260</v>
+        <v>311</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>107</v>
+        <v>117</v>
       </c>
       <c r="D56" s="0" t="s">
-        <v>143</v>
+        <v>117</v>
       </c>
       <c r="E56" s="0" t="s">
         <v>143</v>
@@ -10485,16 +12808,16 @@
         <v>143</v>
       </c>
       <c r="G56" s="0" t="s">
-        <v>143</v>
+        <v>117</v>
       </c>
       <c r="H56" s="0" t="s">
-        <v>107</v>
+        <v>143</v>
       </c>
       <c r="I56" s="0" t="s">
         <v>143</v>
       </c>
       <c r="J56" s="0" t="s">
-        <v>243</v>
+        <v>135</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10502,7 +12825,7 @@
         <v>261</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>262</v>
+        <v>250</v>
       </c>
       <c r="C57" s="0" t="s">
         <v>107</v>
@@ -10526,7 +12849,7 @@
         <v>143</v>
       </c>
       <c r="J57" s="0" t="s">
-        <v>263</v>
+        <v>116</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10534,7 +12857,7 @@
         <v>264</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>265</v>
+        <v>312</v>
       </c>
       <c r="C58" s="0" t="s">
         <v>107</v>
@@ -10566,7 +12889,7 @@
         <v>266</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>267</v>
+        <v>285</v>
       </c>
       <c r="C59" s="0" t="s">
         <v>107</v>
@@ -10595,10 +12918,10 @@
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>268</v>
+        <v>158</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>269</v>
+        <v>252</v>
       </c>
       <c r="C60" s="0" t="s">
         <v>107</v>
@@ -10622,15 +12945,15 @@
         <v>143</v>
       </c>
       <c r="J60" s="0" t="s">
-        <v>263</v>
+        <v>135</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>270</v>
+        <v>179</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>271</v>
+        <v>254</v>
       </c>
       <c r="C61" s="0" t="s">
         <v>107</v>
@@ -10645,30 +12968,30 @@
         <v>143</v>
       </c>
       <c r="G61" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="H61" s="0" t="s">
         <v>107</v>
       </c>
-      <c r="H61" s="0" t="s">
-        <v>143</v>
-      </c>
       <c r="I61" s="0" t="s">
         <v>143</v>
       </c>
       <c r="J61" s="0" t="s">
-        <v>135</v>
+        <v>165</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>272</v>
+        <v>256</v>
       </c>
       <c r="C62" s="0" t="s">
         <v>107</v>
       </c>
       <c r="D62" s="0" t="s">
-        <v>143</v>
+        <v>107</v>
       </c>
       <c r="E62" s="0" t="s">
         <v>143</v>
@@ -10686,15 +13009,15 @@
         <v>143</v>
       </c>
       <c r="J62" s="0" t="s">
-        <v>135</v>
+        <v>257</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>173</v>
+        <v>274</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>273</v>
+        <v>262</v>
       </c>
       <c r="C63" s="0" t="s">
         <v>107</v>
@@ -10718,15 +13041,15 @@
         <v>143</v>
       </c>
       <c r="J63" s="0" t="s">
-        <v>135</v>
+        <v>263</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
       <c r="C64" s="0" t="s">
         <v>107</v>
@@ -10741,30 +13064,30 @@
         <v>143</v>
       </c>
       <c r="G64" s="0" t="s">
-        <v>143</v>
+        <v>107</v>
       </c>
       <c r="H64" s="0" t="s">
-        <v>107</v>
+        <v>143</v>
       </c>
       <c r="I64" s="0" t="s">
         <v>143</v>
       </c>
       <c r="J64" s="0" t="s">
-        <v>116</v>
+        <v>135</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="C65" s="0" t="s">
         <v>107</v>
       </c>
       <c r="D65" s="0" t="s">
-        <v>107</v>
+        <v>143</v>
       </c>
       <c r="E65" s="0" t="s">
         <v>143</v>
@@ -10782,15 +13105,15 @@
         <v>143</v>
       </c>
       <c r="J65" s="0" t="s">
-        <v>199</v>
+        <v>263</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
       <c r="C66" s="0" t="s">
         <v>107</v>
@@ -10814,15 +13137,15 @@
         <v>143</v>
       </c>
       <c r="J66" s="0" t="s">
-        <v>243</v>
+        <v>135</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>281</v>
+        <v>272</v>
       </c>
       <c r="C67" s="0" t="s">
         <v>107</v>
@@ -10843,7 +13166,7 @@
         <v>143</v>
       </c>
       <c r="I67" s="0" t="s">
-        <v>107</v>
+        <v>143</v>
       </c>
       <c r="J67" s="0" t="s">
         <v>135</v>
@@ -10851,10 +13174,10 @@
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>283</v>
+        <v>273</v>
       </c>
       <c r="C68" s="0" t="s">
         <v>107</v>
@@ -10869,48 +13192,144 @@
         <v>143</v>
       </c>
       <c r="G68" s="0" t="s">
-        <v>143</v>
+        <v>107</v>
       </c>
       <c r="H68" s="0" t="s">
-        <v>107</v>
+        <v>143</v>
       </c>
       <c r="I68" s="0" t="s">
         <v>143</v>
       </c>
       <c r="J68" s="0" t="s">
-        <v>116</v>
+        <v>135</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>284</v>
+        <v>313</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>285</v>
+        <v>275</v>
       </c>
       <c r="C69" s="0" t="s">
         <v>107</v>
       </c>
       <c r="D69" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="E69" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="F69" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="G69" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="H69" s="0" t="s">
         <v>107</v>
       </c>
-      <c r="E69" s="0" t="s">
-        <v>143</v>
-      </c>
-      <c r="F69" s="0" t="s">
-        <v>143</v>
-      </c>
-      <c r="G69" s="0" t="s">
+      <c r="I69" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="J69" s="0" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="0" t="s">
+        <v>314</v>
+      </c>
+      <c r="B70" s="0" t="s">
+        <v>277</v>
+      </c>
+      <c r="C70" s="0" t="s">
         <v>107</v>
       </c>
-      <c r="H69" s="0" t="s">
-        <v>143</v>
-      </c>
-      <c r="I69" s="0" t="s">
-        <v>143</v>
-      </c>
-      <c r="J69" s="0" t="s">
-        <v>135</v>
+      <c r="D70" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="E70" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="F70" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="G70" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="H70" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="I70" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="J70" s="0" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="0" t="s">
+        <v>178</v>
+      </c>
+      <c r="B71" s="0" t="s">
+        <v>279</v>
+      </c>
+      <c r="C71" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="D71" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="E71" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="F71" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="G71" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="H71" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="I71" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="J71" s="0" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="0" t="s">
+        <v>315</v>
+      </c>
+      <c r="B72" s="0" t="s">
+        <v>283</v>
+      </c>
+      <c r="C72" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="D72" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="E72" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="F72" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="G72" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="H72" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="I72" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="J72" s="0" t="s">
+        <v>116</v>
       </c>
     </row>
   </sheetData>

</xml_diff>